<commit_message>
count vect; TimeSeries cv
</commit_message>
<xml_diff>
--- a/6_Final_projects/User_identification/kaggle/results.xlsx
+++ b/6_Final_projects/User_identification/kaggle/results.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vlad\Git\Uniholder\Specialization-Yandex-MIPT\6_Final_projects\User_identification\kaggle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16692075\Git\Specialization-Yandex-MIPT\6_Final_projects\User_identification\kaggle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0544BB3-C836-448A-928C-EA62C36EB126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="28995" windowHeight="15675"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>model</t>
   </si>
@@ -39,15 +38,9 @@
     <t>sgdclassifier</t>
   </si>
   <si>
-    <t>bag of sites</t>
-  </si>
-  <si>
     <t>local</t>
   </si>
   <si>
-    <t>0.93362</t>
-  </si>
-  <si>
     <t>roc auc</t>
   </si>
   <si>
@@ -109,13 +102,49 @@
   </si>
   <si>
     <t>0.95965</t>
+  </si>
+  <si>
+    <t>0.85722</t>
+  </si>
+  <si>
+    <t>0.91366</t>
+  </si>
+  <si>
+    <t>~0.85722</t>
+  </si>
+  <si>
+    <t>LogisticRegression</t>
+  </si>
+  <si>
+    <t>0.83341</t>
+  </si>
+  <si>
+    <t>much longer</t>
+  </si>
+  <si>
+    <t>0.90744</t>
+  </si>
+  <si>
+    <t>bag of sites; CountVectorizer</t>
+  </si>
+  <si>
+    <t>bag of sites; csr_matrix</t>
+  </si>
+  <si>
+    <t>bag of sites; CountVectorizer (1, 2)-grams 20k</t>
+  </si>
+  <si>
+    <t>0.91730</t>
+  </si>
+  <si>
+    <t>0.85791</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +158,23 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -152,16 +198,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -174,6 +222,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1588</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1588</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Рисунок 3" descr="http://EDFF839C2394240D7A6C69EF7AF40BB7.dms.sberbank.ru/EDFF839C2394240D7A6C69EF7AF40BB7-86AB11783FAC1265EF5A2B999A130797-FFCEBACF6A69293602AD1A6C013FA945/1.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:link="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1588" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -438,27 +529,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E8:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E8:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17.46484375" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" customWidth="1"/>
-    <col min="9" max="9" width="13.46484375" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="5:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="5:10" x14ac:dyDescent="0.25">
       <c r="H8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="5:9" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,107 +559,152 @@
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="5:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>3</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="5:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E11" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="5:9" x14ac:dyDescent="0.45">
-      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
         <v>3</v>
       </c>
-      <c r="F12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="5:9" x14ac:dyDescent="0.45">
-      <c r="E13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="5:9" x14ac:dyDescent="0.45">
-      <c r="E14" s="1" t="s">
+    </row>
+    <row r="17" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="5:9" x14ac:dyDescent="0.45">
-      <c r="E15" s="1" t="s">
+    <row r="19" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="5:9" x14ac:dyDescent="0.45">
-      <c r="E16" s="1" t="s">
+    <row r="20" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="5:9" x14ac:dyDescent="0.45">
-      <c r="E17" s="1" t="s">
+    <row r="21" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="5:9" x14ac:dyDescent="0.45">
-      <c r="E18" s="1" t="s">
+    <row r="22" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="5:9" x14ac:dyDescent="0.45">
-      <c r="E19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -575,5 +713,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feature engineering + hyperparams
</commit_message>
<xml_diff>
--- a/6_Final_projects/User_identification/kaggle/results.xlsx
+++ b/6_Final_projects/User_identification/kaggle/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
   <si>
     <t>model</t>
   </si>
@@ -191,10 +191,22 @@
     <t>0.91827</t>
   </si>
   <si>
-    <t>0.92010</t>
-  </si>
-  <si>
-    <t>bag of sites; CountVectorizer (1, 2)-grams max-k; morning, day, evening, night, weekday, duration, year_month, is_Sunday</t>
+    <t>bag of sites; CountVectorizer (1, 2)-grams max-k; morning, day, evening, night, weekday, duration, year_month, is_monday, is_wednesday, is_sunday</t>
+  </si>
+  <si>
+    <t>0.93151</t>
+  </si>
+  <si>
+    <t>0.94249</t>
+  </si>
+  <si>
+    <t>bag of sites; CountVectorizer (1, 2)-grams max-k; morning, day, evening,  duration, year, is_monday, is_wednesday, is_sunday</t>
+  </si>
+  <si>
+    <t>0.92982</t>
+  </si>
+  <si>
+    <t>0.94322</t>
   </si>
 </sst>
 </file>
@@ -251,11 +263,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -291,7 +303,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Рисунок 5" descr="http://EDFF839C2394240D7A6C69EF7AF40BB7.dms.sberbank.ru/EDFF839C2394240D7A6C69EF7AF40BB7-86AB11783FAC1265EF5A2B999A130797-AFB9AC55F4E642E8CCA602C997373644/1.png"/>
+        <xdr:cNvPr id="2" name="Рисунок 1" descr="http://EDFF839C2394240D7A6C69EF7AF40BB7.dms.sberbank.ru/EDFF839C2394240D7A6C69EF7AF40BB7-86AB11783FAC1265EF5A2B999A130797-B3BFC84D2366E720731E9E34DE2B3CF0/1.png"/>
         <xdr:cNvPicPr>
           <a:picLocks/>
         </xdr:cNvPicPr>
@@ -580,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A8:J29"/>
+  <dimension ref="A8:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,12 +644,12 @@
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
       <c r="I11" s="1" t="s">
         <v>8</v>
       </c>
@@ -777,7 +789,7 @@
       <c r="E23" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>46</v>
       </c>
       <c r="H23" t="s">
@@ -791,7 +803,7 @@
       <c r="E24" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>50</v>
       </c>
       <c r="H24" t="s">
@@ -808,7 +820,7 @@
       <c r="E25" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="4" t="s">
         <v>53</v>
       </c>
       <c r="H25" t="s">
@@ -816,39 +828,55 @@
       </c>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" t="s">
         <v>56</v>
       </c>
-      <c r="H26" t="s">
-        <v>55</v>
-      </c>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>21</v>
+      <c r="I26" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" t="s">
+        <v>59</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E28" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>